<commit_message>
fixing the game day visuals
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week11.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week11.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,16 +584,16 @@
         <v>7</v>
       </c>
       <c r="K2" t="n">
-        <v>9.1</v>
+        <v>13.6</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Nebraska -4.5</t>
+          <t>UCLA -3.0</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Nebraska -1.5</t>
+          <t>UCLA -3.0</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -605,7 +605,7 @@
         <v>-10.6</v>
       </c>
       <c r="P2" t="n">
-        <v>-1.5</v>
+        <v>3</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
@@ -625,59 +625,59 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>San Diego State</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>18.9</v>
+        <v>27.4</v>
       </c>
       <c r="H3" t="n">
-        <v>27.4</v>
+        <v>27</v>
       </c>
       <c r="I3" t="n">
-        <v>25.81</v>
+        <v>47.19</v>
       </c>
       <c r="J3" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="K3" t="n">
         <v>6.1</v>
       </c>
-      <c r="K3" t="n">
-        <v>6</v>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>West Virginia -6.5</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>West Virginia -6.5</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>San Diego State -8.5</t>
+          <t>West Virginia -0.4</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>-8.5</v>
+        <v>0.4</v>
       </c>
       <c r="P3" t="n">
-        <v>-2.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
@@ -728,16 +728,16 @@
         <v>7.5</v>
       </c>
       <c r="K4" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>USC -16.5</t>
+          <t>USC -15.0</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>USC -14.5</t>
+          <t>USC -15.0</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -749,7 +749,7 @@
         <v>20</v>
       </c>
       <c r="P4" t="n">
-        <v>14.5</v>
+        <v>15</v>
       </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
@@ -800,16 +800,16 @@
         <v>7.7</v>
       </c>
       <c r="K5" t="n">
-        <v>5.199999999999999</v>
+        <v>4.699999999999999</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Virginia -6.5</t>
+          <t>Virginia -7.0</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Virginia -6.5</t>
+          <t>Virginia -7.0</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -821,7 +821,7 @@
         <v>11.7</v>
       </c>
       <c r="P5" t="n">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
@@ -841,7 +841,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -851,49 +851,49 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>34.9</v>
+        <v>43.6</v>
       </c>
       <c r="H6" t="n">
-        <v>23.3</v>
+        <v>10.8</v>
       </c>
       <c r="I6" t="n">
-        <v>74.62</v>
+        <v>96.81999999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>3.8</v>
+        <v>1.9</v>
       </c>
       <c r="K6" t="n">
-        <v>5.1</v>
+        <v>4.299999999999997</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Coastal Carolina -6.5</t>
+          <t>East Carolina -28.5</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Coastal Carolina -6.5</t>
+          <t>East Carolina -28.5</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Coastal Carolina -11.6</t>
+          <t>East Carolina -32.8</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>11.6</v>
+        <v>32.8</v>
       </c>
       <c r="P6" t="n">
-        <v>6.5</v>
+        <v>28.5</v>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
@@ -944,7 +944,7 @@
         <v>4.1</v>
       </c>
       <c r="K7" t="n">
-        <v>4.600000000000001</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Toledo -14</t>
+          <t>Toledo -14.5</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -965,7 +965,7 @@
         <v>18.6</v>
       </c>
       <c r="P7" t="n">
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
@@ -985,59 +985,59 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>26.4</v>
+        <v>34.9</v>
       </c>
       <c r="H8" t="n">
-        <v>28.4</v>
+        <v>23.3</v>
       </c>
       <c r="I8" t="n">
-        <v>40.57</v>
+        <v>74.62</v>
       </c>
       <c r="J8" t="n">
-        <v>9.6</v>
+        <v>3.8</v>
       </c>
       <c r="K8" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -6.5</t>
+          <t>Coastal Carolina -7.5</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -6.5</t>
+          <t>Coastal Carolina -7.5</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -2.1</t>
+          <t>Coastal Carolina -11.6</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>-2.1</v>
+        <v>11.6</v>
       </c>
       <c r="P8" t="n">
-        <v>-6.5</v>
+        <v>7.5</v>
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
@@ -1057,59 +1057,59 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ACC Network</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>21.9</v>
+        <v>26.2</v>
       </c>
       <c r="H9" t="n">
-        <v>30.3</v>
+        <v>27.8</v>
       </c>
       <c r="I9" t="n">
-        <v>25.17</v>
+        <v>40.84</v>
       </c>
       <c r="J9" t="n">
-        <v>4.6</v>
+        <v>9.1</v>
       </c>
       <c r="K9" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Louisiana Tech -4.5</t>
+          <t>Clemson -2.5</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Louisiana Tech -4</t>
+          <t>Clemson -2.5</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Louisiana Tech -8.4</t>
+          <t>Florida State -1.6</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>-8.4</v>
+        <v>-1.6</v>
       </c>
       <c r="P9" t="n">
-        <v>-4</v>
+        <v>2.5</v>
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -1129,59 +1129,59 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>43.6</v>
+        <v>18.9</v>
       </c>
       <c r="H10" t="n">
-        <v>10.8</v>
+        <v>27.4</v>
       </c>
       <c r="I10" t="n">
-        <v>96.81999999999999</v>
+        <v>25.81</v>
       </c>
       <c r="J10" t="n">
-        <v>1.9</v>
+        <v>6.1</v>
       </c>
       <c r="K10" t="n">
-        <v>4.299999999999997</v>
+        <v>4</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>East Carolina -28.5</t>
+          <t>San Diego State -4.5</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>East Carolina -28.5</t>
+          <t>San Diego State -4.5</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>East Carolina -32.8</t>
+          <t>San Diego State -8.5</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>32.8</v>
+        <v>-8.5</v>
       </c>
       <c r="P10" t="n">
-        <v>28.5</v>
+        <v>-4.5</v>
       </c>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
@@ -1201,59 +1201,59 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ACC Network</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>26.2</v>
+        <v>21.9</v>
       </c>
       <c r="H11" t="n">
-        <v>27.8</v>
+        <v>30.3</v>
       </c>
       <c r="I11" t="n">
-        <v>40.84</v>
+        <v>25.17</v>
       </c>
       <c r="J11" t="n">
-        <v>9.1</v>
+        <v>4.6</v>
       </c>
       <c r="K11" t="n">
-        <v>4.1</v>
+        <v>3.9</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Clemson -16.5</t>
+          <t>Louisiana Tech -4.5</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Clemson -2.5</t>
+          <t>Louisiana Tech -4.5</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Florida State -1.6</t>
+          <t>Louisiana Tech -8.4</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>-1.6</v>
+        <v>-8.4</v>
       </c>
       <c r="P11" t="n">
-        <v>2.5</v>
+        <v>-4.5</v>
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
@@ -1273,59 +1273,59 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>TNT</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>27.4</v>
+        <v>26.4</v>
       </c>
       <c r="H12" t="n">
-        <v>27</v>
+        <v>28.4</v>
       </c>
       <c r="I12" t="n">
-        <v>47.19</v>
+        <v>40.57</v>
       </c>
       <c r="J12" t="n">
-        <v>7.6</v>
+        <v>9.6</v>
       </c>
       <c r="K12" t="n">
-        <v>4.1</v>
+        <v>3.9</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>West Virginia -4.5</t>
+          <t>Texas A&amp;M -6.0</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>West Virginia -4.5</t>
+          <t>Texas A&amp;M -6.0</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>West Virginia -0.4</t>
+          <t>Texas A&amp;M -2.1</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>0.4</v>
+        <v>-2.1</v>
       </c>
       <c r="P12" t="n">
-        <v>4.5</v>
+        <v>-6</v>
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
@@ -1345,59 +1345,59 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>25</v>
+        <v>35.4</v>
       </c>
       <c r="H13" t="n">
-        <v>22.8</v>
+        <v>25.6</v>
       </c>
       <c r="I13" t="n">
-        <v>51.12</v>
+        <v>70.83</v>
       </c>
       <c r="J13" t="n">
-        <v>8.800000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="K13" t="n">
-        <v>3.6</v>
+        <v>3.300000000000001</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Houston -2.5</t>
+          <t>Memphis -6.5</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Houston -1.5</t>
+          <t>Memphis -6.5</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>UCF -2.1</t>
+          <t>Memphis -9.8</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>2.1</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="P13" t="n">
-        <v>-1.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1413,63 +1413,63 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45969</v>
+        <v>45965</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>32.5</v>
+        <v>30.4</v>
       </c>
       <c r="H14" t="n">
-        <v>25.9</v>
+        <v>17.4</v>
       </c>
       <c r="I14" t="n">
-        <v>63.68</v>
+        <v>77.67</v>
       </c>
       <c r="J14" t="n">
-        <v>8.9</v>
+        <v>2.4</v>
       </c>
       <c r="K14" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Arizona -3.5</t>
+          <t>Akron -10.0</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Arizona -3.5</t>
+          <t>Akron -10.0</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Arizona -6.6</t>
+          <t>Akron -13.0</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>6.6</v>
+        <v>13</v>
       </c>
       <c r="P14" t="n">
-        <v>3.5</v>
+        <v>10</v>
       </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1485,11 +1485,11 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45965</v>
+        <v>45969</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1499,49 +1499,49 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>30.4</v>
+        <v>28.1</v>
       </c>
       <c r="H15" t="n">
-        <v>17.4</v>
+        <v>33.7</v>
       </c>
       <c r="I15" t="n">
-        <v>77.67</v>
+        <v>31.54</v>
       </c>
       <c r="J15" t="n">
-        <v>2.4</v>
+        <v>7.6</v>
       </c>
       <c r="K15" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Akron -9.5</t>
+          <t>Duke -8.5</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Akron -10</t>
+          <t>Duke -8.5</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Akron -13.0</t>
+          <t>Duke -5.6</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>13</v>
+        <v>-5.6</v>
       </c>
       <c r="P15" t="n">
-        <v>10</v>
+        <v>-8.5</v>
       </c>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
@@ -1557,7 +1557,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45969</v>
+        <v>45966</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1566,54 +1566,54 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Kent State</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>35.8</v>
+        <v>28.2</v>
       </c>
       <c r="H16" t="n">
-        <v>15.4</v>
+        <v>23</v>
       </c>
       <c r="I16" t="n">
-        <v>88.42</v>
+        <v>59.7</v>
       </c>
       <c r="J16" t="n">
-        <v>6.1</v>
+        <v>4</v>
       </c>
       <c r="K16" t="n">
-        <v>2.899999999999999</v>
+        <v>2.8</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Louisville -17.5</t>
+          <t>Ball State -2.5</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Louisville -17.5</t>
+          <t>Ball State -2.5</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Louisville -20.4</t>
+          <t>Ball State -5.3</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>20.4</v>
+        <v>5.3</v>
       </c>
       <c r="P16" t="n">
-        <v>17.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
@@ -1629,63 +1629,63 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8:00 PM</t>
+          <t>3:30 PM</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>35.4</v>
+        <v>26.2</v>
       </c>
       <c r="H17" t="n">
-        <v>25.6</v>
+        <v>19.8</v>
       </c>
       <c r="I17" t="n">
-        <v>70.83</v>
+        <v>62.11</v>
       </c>
       <c r="J17" t="n">
-        <v>8.1</v>
+        <v>6.8</v>
       </c>
       <c r="K17" t="n">
-        <v>2.800000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Memphis -4.5</t>
+          <t>North Carolina -9.0</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Memphis -7</t>
+          <t>North Carolina -9.0</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Memphis -9.8</t>
+          <t>North Carolina -6.3</t>
         </is>
       </c>
       <c r="O17" t="n">
-        <v>9.800000000000001</v>
+        <v>6.3</v>
       </c>
       <c r="P17" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -1701,63 +1701,63 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45966</v>
+        <v>45969</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Kent State</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>28.2</v>
+        <v>18.5</v>
       </c>
       <c r="H18" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I18" t="n">
-        <v>59.7</v>
+        <v>23.52</v>
       </c>
       <c r="J18" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="K18" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Ball State -3.0</t>
+          <t>Kennesaw State -7.0</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Ball State -2.5</t>
+          <t>Kennesaw State -7.0</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Ball State -5.3</t>
+          <t>Kennesaw State -9.5</t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>5.3</v>
+        <v>-9.5</v>
       </c>
       <c r="P18" t="n">
-        <v>2.5</v>
+        <v>-7</v>
       </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
@@ -1777,59 +1777,59 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>ACC Network</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H19" t="n">
-        <v>17.4</v>
+        <v>34.4</v>
       </c>
       <c r="I19" t="n">
-        <v>93.68000000000001</v>
+        <v>15.35</v>
       </c>
       <c r="J19" t="n">
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="K19" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Notre Dame -24.5</t>
+          <t>SMU -12.0</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Notre Dame -24.5</t>
+          <t>SMU -12.0</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Notre Dame -26.5</t>
+          <t>SMU -14.5</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>26.5</v>
+        <v>-14.5</v>
       </c>
       <c r="P19" t="n">
-        <v>24.5</v>
+        <v>-12</v>
       </c>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
@@ -1849,59 +1849,59 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>30.2</v>
+        <v>34</v>
       </c>
       <c r="H20" t="n">
-        <v>21.6</v>
+        <v>20.6</v>
       </c>
       <c r="I20" t="n">
-        <v>67.73</v>
+        <v>78.44</v>
       </c>
       <c r="J20" t="n">
-        <v>5.4</v>
+        <v>4.2</v>
       </c>
       <c r="K20" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Liberty -6.5</t>
+          <t>Utah State -11.0</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Liberty -6.5</t>
+          <t>Utah State -11.0</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Liberty -8.5</t>
+          <t>Utah State -13.4</t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>8.5</v>
+        <v>13.4</v>
       </c>
       <c r="P20" t="n">
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
@@ -1917,63 +1917,63 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45969</v>
+        <v>45968</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>25.9</v>
+        <v>18</v>
       </c>
       <c r="H21" t="n">
-        <v>25.7</v>
+        <v>31.4</v>
       </c>
       <c r="I21" t="n">
-        <v>46.64</v>
+        <v>16.87</v>
       </c>
       <c r="J21" t="n">
-        <v>4.5</v>
+        <v>6.8</v>
       </c>
       <c r="K21" t="n">
-        <v>1.7</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Florida International -1.5</t>
+          <t>Washington -11.0</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Florida International -1.5</t>
+          <t>Washington -11.0</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Middle Tennessee -0.2</t>
+          <t>Washington -13.3</t>
         </is>
       </c>
       <c r="O21" t="n">
-        <v>0.2</v>
+        <v>-13.3</v>
       </c>
       <c r="P21" t="n">
-        <v>-1.5</v>
+        <v>-11</v>
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
@@ -1993,59 +1993,59 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>30.4</v>
+        <v>23.4</v>
       </c>
       <c r="H22" t="n">
-        <v>27.4</v>
+        <v>33</v>
       </c>
       <c r="I22" t="n">
-        <v>54.48</v>
+        <v>23.92</v>
       </c>
       <c r="J22" t="n">
-        <v>5.7</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="K22" t="n">
-        <v>1.6</v>
+        <v>2.199999999999999</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Rice -4.5</t>
+          <t>Georgia -7.5</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Rice -4.5</t>
+          <t>Georgia -7.5</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Rice -2.9</t>
+          <t>Georgia -9.7</t>
         </is>
       </c>
       <c r="O22" t="n">
-        <v>2.9</v>
+        <v>-9.699999999999999</v>
       </c>
       <c r="P22" t="n">
-        <v>4.5</v>
+        <v>-7.5</v>
       </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
@@ -2061,63 +2061,63 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45965</v>
+        <v>45968</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H23" t="n">
-        <v>21.8</v>
+        <v>22.8</v>
       </c>
       <c r="I23" t="n">
-        <v>58.89</v>
+        <v>51.12</v>
       </c>
       <c r="J23" t="n">
-        <v>7.3</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="K23" t="n">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Ohio -3.5</t>
+          <t>UCF --0.0</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Ohio -3.5</t>
+          <t>Houston -0.0</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Ohio -5.1</t>
+          <t>UCF -2.1</t>
         </is>
       </c>
       <c r="O23" t="n">
-        <v>5.1</v>
+        <v>2.1</v>
       </c>
       <c r="P23" t="n">
-        <v>3.5</v>
+        <v>-0</v>
       </c>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
@@ -2137,59 +2137,59 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>8:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>28.5</v>
+        <v>25.4</v>
       </c>
       <c r="H24" t="n">
-        <v>33.4</v>
+        <v>29.2</v>
       </c>
       <c r="I24" t="n">
-        <v>34.52</v>
+        <v>35.54</v>
       </c>
       <c r="J24" t="n">
         <v>5.8</v>
       </c>
       <c r="K24" t="n">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>UNLV -6.5</t>
+          <t>Southern Miss -6.0</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>UNLV -6.5</t>
+          <t>Southern Miss -6.0</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>UNLV -4.9</t>
+          <t>Southern Miss -3.9</t>
         </is>
       </c>
       <c r="O24" t="n">
-        <v>-4.9</v>
+        <v>-3.9</v>
       </c>
       <c r="P24" t="n">
-        <v>-6.5</v>
+        <v>-6</v>
       </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
@@ -2209,59 +2209,59 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>BTN</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>10.5</v>
+        <v>44</v>
       </c>
       <c r="H25" t="n">
-        <v>40.3</v>
+        <v>17.4</v>
       </c>
       <c r="I25" t="n">
-        <v>3.22</v>
+        <v>93.68000000000001</v>
       </c>
       <c r="J25" t="n">
-        <v>5.1</v>
+        <v>6.3</v>
       </c>
       <c r="K25" t="n">
-        <v>1.300000000000001</v>
+        <v>2</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Ohio State -28.5</t>
+          <t>Notre Dame -24.5</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Ohio State -28.5</t>
+          <t>Notre Dame -24.5</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Ohio State -29.8</t>
+          <t>Notre Dame -26.5</t>
         </is>
       </c>
       <c r="O25" t="n">
-        <v>-29.8</v>
+        <v>26.5</v>
       </c>
       <c r="P25" t="n">
-        <v>-28.5</v>
+        <v>24.5</v>
       </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -2281,59 +2281,59 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>3:30 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>California</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>26.2</v>
+        <v>35.8</v>
       </c>
       <c r="H26" t="n">
-        <v>19.8</v>
+        <v>15.4</v>
       </c>
       <c r="I26" t="n">
-        <v>62.11</v>
+        <v>88.42</v>
       </c>
       <c r="J26" t="n">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="K26" t="n">
-        <v>1.2</v>
+        <v>1.899999999999999</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>North Carolina -7.5</t>
+          <t>Louisville -18.5</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>North Carolina -7.5</t>
+          <t>Louisville -18.5</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>North Carolina -6.3</t>
+          <t>Louisville -20.4</t>
         </is>
       </c>
       <c r="O26" t="n">
-        <v>6.3</v>
+        <v>20.4</v>
       </c>
       <c r="P26" t="n">
-        <v>7.5</v>
+        <v>18.5</v>
       </c>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
@@ -2349,63 +2349,63 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45967</v>
+        <v>45969</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>33</v>
+        <v>29.6</v>
       </c>
       <c r="H27" t="n">
-        <v>28.8</v>
+        <v>24.8</v>
       </c>
       <c r="I27" t="n">
-        <v>57.52</v>
+        <v>58.35</v>
       </c>
       <c r="J27" t="n">
-        <v>6.3</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K27" t="n">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>App State -5.5</t>
+          <t>TCU -6.5</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>App State -5.5</t>
+          <t>TCU -6.5</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>App State -4.3</t>
+          <t>TCU -4.8</t>
         </is>
       </c>
       <c r="O27" t="n">
-        <v>4.3</v>
+        <v>4.8</v>
       </c>
       <c r="P27" t="n">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
@@ -2421,63 +2421,63 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45969</v>
+        <v>45967</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>23.4</v>
+        <v>33</v>
       </c>
       <c r="H28" t="n">
-        <v>33</v>
+        <v>28.8</v>
       </c>
       <c r="I28" t="n">
-        <v>23.92</v>
+        <v>57.52</v>
       </c>
       <c r="J28" t="n">
-        <v>8.699999999999999</v>
+        <v>6.3</v>
       </c>
       <c r="K28" t="n">
-        <v>1.199999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Georgia -9.5</t>
+          <t>App State -6.0</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Georgia -8.5</t>
+          <t>App State -6.0</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Georgia -9.7</t>
+          <t>App State -4.3</t>
         </is>
       </c>
       <c r="O28" t="n">
-        <v>-9.699999999999999</v>
+        <v>4.3</v>
       </c>
       <c r="P28" t="n">
-        <v>-8.5</v>
+        <v>6</v>
       </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
@@ -2493,63 +2493,63 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45969</v>
+        <v>45965</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1:30 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>27.5</v>
+        <v>27</v>
       </c>
       <c r="H29" t="n">
-        <v>27.1</v>
+        <v>21.8</v>
       </c>
       <c r="I29" t="n">
-        <v>47.47</v>
+        <v>58.89</v>
       </c>
       <c r="J29" t="n">
-        <v>8.300000000000001</v>
+        <v>7.3</v>
       </c>
       <c r="K29" t="n">
-        <v>1.1</v>
+        <v>1.6</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Rutgers -1.5</t>
+          <t>Ohio -3.5</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Rutgers -1.5</t>
+          <t>Ohio -3.5</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Rutgers -0.4</t>
+          <t>Ohio -5.1</t>
         </is>
       </c>
       <c r="O29" t="n">
-        <v>0.4</v>
+        <v>5.1</v>
       </c>
       <c r="P29" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
@@ -2565,63 +2565,63 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45969</v>
+        <v>45968</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>30.8</v>
+        <v>19.8</v>
       </c>
       <c r="H30" t="n">
-        <v>32.8</v>
+        <v>27.2</v>
       </c>
       <c r="I30" t="n">
-        <v>41.65</v>
+        <v>27.57</v>
       </c>
       <c r="J30" t="n">
-        <v>6.1</v>
+        <v>9.4</v>
       </c>
       <c r="K30" t="n">
-        <v>1.1</v>
+        <v>1.5</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Texas State -3.0</t>
+          <t>Oregon -6.0</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Texas State -3</t>
+          <t>Oregon -6.0</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Texas State -1.9</t>
+          <t>Oregon -7.5</t>
         </is>
       </c>
       <c r="O30" t="n">
-        <v>-1.9</v>
+        <v>-7.5</v>
       </c>
       <c r="P30" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
@@ -2641,59 +2641,59 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>29.3</v>
+        <v>36.6</v>
       </c>
       <c r="H31" t="n">
-        <v>21.3</v>
+        <v>16.7</v>
       </c>
       <c r="I31" t="n">
-        <v>66.73999999999999</v>
+        <v>88.19</v>
       </c>
       <c r="J31" t="n">
-        <v>9.300000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="K31" t="n">
-        <v>1</v>
+        <v>1.399999999999999</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Vanderbilt -5.5</t>
+          <t>Oregon State -18.5</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Vanderbilt -7</t>
+          <t>Oregon State -18.5</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Vanderbilt -8.0</t>
+          <t>Oregon State -19.9</t>
         </is>
       </c>
       <c r="O31" t="n">
-        <v>8</v>
+        <v>19.9</v>
       </c>
       <c r="P31" t="n">
-        <v>7</v>
+        <v>18.5</v>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
@@ -2718,54 +2718,54 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>BTN</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>26.2</v>
+        <v>10.5</v>
       </c>
       <c r="H32" t="n">
-        <v>25.6</v>
+        <v>40.3</v>
       </c>
       <c r="I32" t="n">
-        <v>47.47</v>
+        <v>3.22</v>
       </c>
       <c r="J32" t="n">
-        <v>5</v>
+        <v>5.1</v>
       </c>
       <c r="K32" t="n">
-        <v>1</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Eastern Michigan -1.5</t>
+          <t>Ohio State -28.5</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Eastern Michigan -1.5</t>
+          <t>Ohio State -28.5</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Eastern Michigan -0.5</t>
+          <t>Ohio State -29.8</t>
         </is>
       </c>
       <c r="O32" t="n">
-        <v>0.5</v>
+        <v>-29.8</v>
       </c>
       <c r="P32" t="n">
-        <v>1.5</v>
+        <v>-28.5</v>
       </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
@@ -2785,59 +2785,59 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>20.9</v>
+        <v>25.9</v>
       </c>
       <c r="H33" t="n">
-        <v>25.4</v>
+        <v>25.7</v>
       </c>
       <c r="I33" t="n">
-        <v>34.52</v>
+        <v>46.64</v>
       </c>
       <c r="J33" t="n">
-        <v>8.4</v>
+        <v>4.5</v>
       </c>
       <c r="K33" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Florida -4.5</t>
+          <t>Florida International -1.0</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Florida -3.5</t>
+          <t>Florida International -1.0</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Florida -4.5</t>
+          <t>Middle Tennessee -0.2</t>
         </is>
       </c>
       <c r="O33" t="n">
-        <v>-4.5</v>
+        <v>0.2</v>
       </c>
       <c r="P33" t="n">
-        <v>-3.5</v>
+        <v>-1</v>
       </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
@@ -2853,63 +2853,63 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>8:30 PM</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>19.8</v>
+        <v>28.5</v>
       </c>
       <c r="H34" t="n">
-        <v>27.2</v>
+        <v>33.4</v>
       </c>
       <c r="I34" t="n">
-        <v>27.57</v>
+        <v>34.52</v>
       </c>
       <c r="J34" t="n">
-        <v>9.4</v>
+        <v>5.8</v>
       </c>
       <c r="K34" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Oregon -7.5</t>
+          <t>UNLV -6.0</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Oregon -6.5</t>
+          <t>UNLV -6.0</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Oregon -7.5</t>
+          <t>UNLV -4.9</t>
         </is>
       </c>
       <c r="O34" t="n">
-        <v>-7.5</v>
+        <v>-4.9</v>
       </c>
       <c r="P34" t="n">
-        <v>-6.5</v>
+        <v>-6</v>
       </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
@@ -2929,59 +2929,59 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ACC Network</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>20</v>
+        <v>30.9</v>
       </c>
       <c r="H35" t="n">
-        <v>34.4</v>
+        <v>18.9</v>
       </c>
       <c r="I35" t="n">
-        <v>15.35</v>
+        <v>75.04000000000001</v>
       </c>
       <c r="J35" t="n">
-        <v>5.4</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K35" t="n">
         <v>1</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>SMU -13.5</t>
+          <t>Alabama -11.0</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>SMU -13.5</t>
+          <t>Alabama -11.0</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>SMU -14.5</t>
+          <t>Alabama -12.0</t>
         </is>
       </c>
       <c r="O35" t="n">
-        <v>-14.5</v>
+        <v>12</v>
       </c>
       <c r="P35" t="n">
-        <v>-13.5</v>
+        <v>11</v>
       </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3011,49 +3011,49 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>24</v>
+        <v>26.2</v>
       </c>
       <c r="H36" t="n">
-        <v>26.2</v>
+        <v>25.6</v>
       </c>
       <c r="I36" t="n">
-        <v>41.38</v>
+        <v>47.47</v>
       </c>
       <c r="J36" t="n">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="K36" t="n">
-        <v>0.7999999999999998</v>
+        <v>1</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Jacksonville State -1.5</t>
+          <t>Eastern Michigan -1.5</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Jacksonville State -1.5</t>
+          <t>Eastern Michigan -1.5</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Jacksonville State -2.3</t>
+          <t>Eastern Michigan -0.5</t>
         </is>
       </c>
       <c r="O36" t="n">
-        <v>-2.3</v>
+        <v>0.5</v>
       </c>
       <c r="P36" t="n">
-        <v>-1.5</v>
+        <v>1.5</v>
       </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
@@ -3073,59 +3073,59 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>31</v>
+        <v>20.9</v>
       </c>
       <c r="H37" t="n">
-        <v>23.8</v>
+        <v>25.4</v>
       </c>
       <c r="I37" t="n">
-        <v>63.68</v>
+        <v>34.52</v>
       </c>
       <c r="J37" t="n">
-        <v>7</v>
+        <v>8.4</v>
       </c>
       <c r="K37" t="n">
-        <v>0.7000000000000002</v>
+        <v>1</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Army -6.5</t>
+          <t>Florida -3.5</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Army -6.5</t>
+          <t>Florida -3.5</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Army -7.2</t>
+          <t>Florida -4.5</t>
         </is>
       </c>
       <c r="O37" t="n">
-        <v>7.2</v>
+        <v>-4.5</v>
       </c>
       <c r="P37" t="n">
-        <v>6.5</v>
+        <v>-3.5</v>
       </c>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
@@ -3145,59 +3145,59 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>29.6</v>
+        <v>31.2</v>
       </c>
       <c r="H38" t="n">
-        <v>24.8</v>
+        <v>21.5</v>
       </c>
       <c r="I38" t="n">
-        <v>58.35</v>
+        <v>70.37</v>
       </c>
       <c r="J38" t="n">
-        <v>9.199999999999999</v>
+        <v>9.5</v>
       </c>
       <c r="K38" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>TCU -3.0</t>
+          <t>Texas Tech -10.5</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>TCU -5.5</t>
+          <t>Texas Tech -10.5</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>TCU -4.8</t>
+          <t>Texas Tech -9.7</t>
         </is>
       </c>
       <c r="O38" t="n">
-        <v>4.8</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="P38" t="n">
-        <v>5.5</v>
+        <v>10.5</v>
       </c>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
@@ -3213,63 +3213,63 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>20</v>
+        <v>31.4</v>
       </c>
       <c r="H39" t="n">
-        <v>32.8</v>
+        <v>26</v>
       </c>
       <c r="I39" t="n">
-        <v>17.67</v>
+        <v>59.43</v>
       </c>
       <c r="J39" t="n">
-        <v>9</v>
+        <v>5.6</v>
       </c>
       <c r="K39" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Indiana -11.5</t>
+          <t>Florida Atlantic -4.5</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Indiana -13.5</t>
+          <t>Florida Atlantic -4.5</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Indiana -12.8</t>
+          <t>Florida Atlantic -5.3</t>
         </is>
       </c>
       <c r="O39" t="n">
-        <v>-12.8</v>
+        <v>5.3</v>
       </c>
       <c r="P39" t="n">
-        <v>-13.5</v>
+        <v>4.5</v>
       </c>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
@@ -3289,59 +3289,59 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>34.3</v>
+        <v>24</v>
       </c>
       <c r="H40" t="n">
-        <v>31.2</v>
+        <v>26.2</v>
       </c>
       <c r="I40" t="n">
-        <v>53.92</v>
+        <v>41.38</v>
       </c>
       <c r="J40" t="n">
-        <v>7.1</v>
+        <v>5.2</v>
       </c>
       <c r="K40" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>San José State -2.5</t>
+          <t>Jacksonville State -1.5</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>San José State -2.5</t>
+          <t>Jacksonville State -1.5</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>San José State -3.1</t>
+          <t>Jacksonville State -2.3</t>
         </is>
       </c>
       <c r="O40" t="n">
-        <v>3.1</v>
+        <v>-2.3</v>
       </c>
       <c r="P40" t="n">
-        <v>2.5</v>
+        <v>-1.5</v>
       </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
@@ -3361,59 +3361,59 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Army</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>30.9</v>
+        <v>31</v>
       </c>
       <c r="H41" t="n">
-        <v>18.9</v>
+        <v>23.8</v>
       </c>
       <c r="I41" t="n">
-        <v>75.04000000000001</v>
+        <v>63.68</v>
       </c>
       <c r="J41" t="n">
-        <v>9.300000000000001</v>
+        <v>7</v>
       </c>
       <c r="K41" t="n">
-        <v>0.5</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Alabama -5.5</t>
+          <t>Army -6.5</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Alabama -11.5</t>
+          <t>Army -6.5</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Alabama -12.0</t>
+          <t>Army -7.2</t>
         </is>
       </c>
       <c r="O41" t="n">
-        <v>12</v>
+        <v>7.2</v>
       </c>
       <c r="P41" t="n">
-        <v>11.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
@@ -3429,63 +3429,63 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>37.8</v>
+        <v>20</v>
       </c>
       <c r="H42" t="n">
-        <v>25</v>
+        <v>32.8</v>
       </c>
       <c r="I42" t="n">
-        <v>77.48</v>
+        <v>17.67</v>
       </c>
       <c r="J42" t="n">
-        <v>7.6</v>
+        <v>9</v>
       </c>
       <c r="K42" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>South Florida -12.5</t>
+          <t>Indiana -13.5</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>South Florida -12.5</t>
+          <t>Indiana -13.5</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>South Florida -12.8</t>
+          <t>Indiana -12.8</t>
         </is>
       </c>
       <c r="O42" t="n">
-        <v>12.8</v>
+        <v>-12.8</v>
       </c>
       <c r="P42" t="n">
-        <v>12.5</v>
+        <v>-13.5</v>
       </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
@@ -3505,59 +3505,59 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>22.4</v>
+        <v>41</v>
       </c>
       <c r="H43" t="n">
-        <v>35.2</v>
+        <v>12.4</v>
       </c>
       <c r="I43" t="n">
-        <v>17.83</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="J43" t="n">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
       <c r="K43" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.6000000000000014</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>James Madison -12.5</t>
+          <t>Miami -28.0</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>James Madison -12.5</t>
+          <t>Miami -28.0</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>James Madison -12.8</t>
+          <t>Miami -28.6</t>
         </is>
       </c>
       <c r="O43" t="n">
-        <v>-12.8</v>
+        <v>28.6</v>
       </c>
       <c r="P43" t="n">
-        <v>-12.5</v>
+        <v>28</v>
       </c>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3587,49 +3587,49 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>31.4</v>
+        <v>30.8</v>
       </c>
       <c r="H44" t="n">
-        <v>26</v>
+        <v>32.8</v>
       </c>
       <c r="I44" t="n">
-        <v>59.43</v>
+        <v>41.65</v>
       </c>
       <c r="J44" t="n">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
       <c r="K44" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Florida Atlantic -5.5</t>
+          <t>Texas State -2.5</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Florida Atlantic -5.5</t>
+          <t>Texas State -2.5</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>Florida Atlantic -5.3</t>
+          <t>Texas State -1.9</t>
         </is>
       </c>
       <c r="O44" t="n">
-        <v>5.3</v>
+        <v>-1.9</v>
       </c>
       <c r="P44" t="n">
-        <v>5.5</v>
+        <v>-2.5</v>
       </c>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
@@ -3649,59 +3649,59 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>1:30 PM</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>31.2</v>
+        <v>27.5</v>
       </c>
       <c r="H45" t="n">
-        <v>21.5</v>
+        <v>27.1</v>
       </c>
       <c r="I45" t="n">
-        <v>70.37</v>
+        <v>47.47</v>
       </c>
       <c r="J45" t="n">
-        <v>9.5</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="K45" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.6</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Texas Tech -8.5</t>
+          <t>Rutgers -1.0</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Texas Tech -9.5</t>
+          <t>Rutgers -1.0</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Texas Tech -9.7</t>
+          <t>Rutgers -0.4</t>
         </is>
       </c>
       <c r="O45" t="n">
-        <v>9.699999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="P45" t="n">
-        <v>9.5</v>
+        <v>1</v>
       </c>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
@@ -3717,63 +3717,63 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>18</v>
+        <v>32.5</v>
       </c>
       <c r="H46" t="n">
-        <v>31.4</v>
+        <v>25.9</v>
       </c>
       <c r="I46" t="n">
-        <v>16.87</v>
+        <v>63.68</v>
       </c>
       <c r="J46" t="n">
-        <v>6.8</v>
+        <v>8.9</v>
       </c>
       <c r="K46" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.5999999999999996</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Washington -13.5</t>
+          <t>Arizona -6.0</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Washington -13.5</t>
+          <t>Arizona -6.0</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Washington -13.3</t>
+          <t>Arizona -6.6</t>
         </is>
       </c>
       <c r="O46" t="n">
-        <v>-13.3</v>
+        <v>6.6</v>
       </c>
       <c r="P46" t="n">
-        <v>-13.5</v>
+        <v>6</v>
       </c>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
@@ -3793,59 +3793,59 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>41</v>
+        <v>30.2</v>
       </c>
       <c r="H47" t="n">
-        <v>12.4</v>
+        <v>21.6</v>
       </c>
       <c r="I47" t="n">
-        <v>94.98999999999999</v>
+        <v>67.73</v>
       </c>
       <c r="J47" t="n">
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="K47" t="n">
-        <v>0.1000000000000014</v>
+        <v>0.5</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Miami -28.5</t>
+          <t>Liberty -8.0</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Miami -28.5</t>
+          <t>Liberty -8.0</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Miami -28.6</t>
+          <t>Liberty -8.5</t>
         </is>
       </c>
       <c r="O47" t="n">
-        <v>28.6</v>
+        <v>8.5</v>
       </c>
       <c r="P47" t="n">
-        <v>28.5</v>
+        <v>8</v>
       </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
@@ -3856,6 +3856,366 @@
         <v>0</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>3:00 PM</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>SEC Network</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Vanderbilt</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Auburn</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="H48" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="I48" t="n">
+        <v>66.73999999999999</v>
+      </c>
+      <c r="J48" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Vanderbilt -7.5</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>Vanderbilt -7.5</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Vanderbilt -8.0</t>
+        </is>
+      </c>
+      <c r="O48" t="n">
+        <v>8</v>
+      </c>
+      <c r="P48" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>5:00 PM</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>FS1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>San José State</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Air Force</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="H49" t="n">
+        <v>31.2</v>
+      </c>
+      <c r="I49" t="n">
+        <v>53.92</v>
+      </c>
+      <c r="J49" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.3999999999999999</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>San José State -3.5</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>San José State -3.5</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>San José State -3.1</t>
+        </is>
+      </c>
+      <c r="O49" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="P49" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>11:00 AM</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>ESPN2</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Marshall</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>James Madison</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="H50" t="n">
+        <v>35.2</v>
+      </c>
+      <c r="I50" t="n">
+        <v>17.83</v>
+      </c>
+      <c r="J50" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.3000000000000007</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>James Madison -12.5</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>James Madison -12.5</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>James Madison -12.8</t>
+        </is>
+      </c>
+      <c r="O50" t="n">
+        <v>-12.8</v>
+      </c>
+      <c r="P50" t="n">
+        <v>-12.5</v>
+      </c>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>45967</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>6:30 PM</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>ESPN</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>South Florida</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>UTSA</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>37.8</v>
+      </c>
+      <c r="H51" t="n">
+        <v>25</v>
+      </c>
+      <c r="I51" t="n">
+        <v>77.48</v>
+      </c>
+      <c r="J51" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.1999999999999993</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>South Florida -13.0</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>South Florida -13.0</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>South Florida -12.8</t>
+        </is>
+      </c>
+      <c r="O51" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="P51" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1:00 PM</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>ESPN+</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>UAB</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="H52" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="I52" t="n">
+        <v>54.48</v>
+      </c>
+      <c r="J52" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.1000000000000001</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Rice -3.0</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Rice -3.0</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Rice -2.9</t>
+        </is>
+      </c>
+      <c r="O52" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="P52" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new team profiles for both softball and baseball
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week11.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week11.xlsx
@@ -584,7 +584,7 @@
         <v>7</v>
       </c>
       <c r="K2" t="n">
-        <v>13.1</v>
+        <v>12.1</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -593,7 +593,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>UCLA -2.5</t>
+          <t>UCLA -1.5</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -605,7 +605,7 @@
         <v>-10.6</v>
       </c>
       <c r="P2" t="n">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
@@ -769,59 +769,59 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>30</v>
+        <v>26.4</v>
       </c>
       <c r="H5" t="n">
-        <v>18.2</v>
+        <v>28.4</v>
       </c>
       <c r="I5" t="n">
-        <v>74.83</v>
+        <v>40.57</v>
       </c>
       <c r="J5" t="n">
-        <v>7.7</v>
+        <v>9.6</v>
       </c>
       <c r="K5" t="n">
-        <v>5.199999999999999</v>
+        <v>4.9</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Virginia -7.0</t>
+          <t>Texas A&amp;M -6.0</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Virginia -6.5</t>
+          <t>Texas A&amp;M -7.0</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Virginia -11.7</t>
+          <t>Texas A&amp;M -2.1</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>11.7</v>
+        <v>-2.1</v>
       </c>
       <c r="P5" t="n">
-        <v>6.5</v>
+        <v>-7</v>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
@@ -841,59 +841,59 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>26.4</v>
+        <v>30</v>
       </c>
       <c r="H6" t="n">
-        <v>28.4</v>
+        <v>18.2</v>
       </c>
       <c r="I6" t="n">
-        <v>40.57</v>
+        <v>74.83</v>
       </c>
       <c r="J6" t="n">
-        <v>9.6</v>
+        <v>7.7</v>
       </c>
       <c r="K6" t="n">
-        <v>4.9</v>
+        <v>4.699999999999999</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -6.0</t>
+          <t>Virginia -7.0</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -7.0</t>
+          <t>Virginia -7.0</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -2.1</t>
+          <t>Virginia -11.7</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>-2.1</v>
+        <v>11.7</v>
       </c>
       <c r="P6" t="n">
-        <v>-7</v>
+        <v>7</v>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
@@ -913,59 +913,59 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ACC Network</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>26.2</v>
+        <v>43.6</v>
       </c>
       <c r="H7" t="n">
-        <v>27.8</v>
+        <v>10.8</v>
       </c>
       <c r="I7" t="n">
-        <v>40.84</v>
+        <v>96.81999999999999</v>
       </c>
       <c r="J7" t="n">
-        <v>9.1</v>
+        <v>1.9</v>
       </c>
       <c r="K7" t="n">
-        <v>4.6</v>
+        <v>4.299999999999997</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Clemson -2.5</t>
+          <t>East Carolina -28.5</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Clemson -3.0</t>
+          <t>East Carolina -28.5</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Florida State -1.6</t>
+          <t>East Carolina -32.8</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>-1.6</v>
+        <v>32.8</v>
       </c>
       <c r="P7" t="n">
-        <v>3</v>
+        <v>28.5</v>
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
@@ -981,63 +981,63 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45969</v>
+        <v>45966</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Northern Illinois</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>43.6</v>
+        <v>28.5</v>
       </c>
       <c r="H8" t="n">
-        <v>10.8</v>
+        <v>9.9</v>
       </c>
       <c r="I8" t="n">
-        <v>96.81999999999999</v>
+        <v>86.58</v>
       </c>
       <c r="J8" t="n">
-        <v>1.9</v>
+        <v>4.1</v>
       </c>
       <c r="K8" t="n">
-        <v>4.299999999999997</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>East Carolina -28.5</t>
+          <t>Toledo -14.5</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>East Carolina -28.5</t>
+          <t>Toledo -14.5</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>East Carolina -32.8</t>
+          <t>Toledo -18.6</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>32.8</v>
+        <v>18.6</v>
       </c>
       <c r="P8" t="n">
-        <v>28.5</v>
+        <v>14.5</v>
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
@@ -1053,63 +1053,63 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45966</v>
+        <v>45969</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Northern Illinois</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>28.5</v>
+        <v>34.9</v>
       </c>
       <c r="H9" t="n">
-        <v>9.9</v>
+        <v>23.3</v>
       </c>
       <c r="I9" t="n">
-        <v>86.58</v>
+        <v>74.62</v>
       </c>
       <c r="J9" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="K9" t="n">
         <v>4.1</v>
       </c>
-      <c r="K9" t="n">
-        <v>4.100000000000001</v>
-      </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Toledo -14.5</t>
+          <t>Coastal Carolina -7.5</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Toledo -14.5</t>
+          <t>Coastal Carolina -7.5</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Toledo -18.6</t>
+          <t>Coastal Carolina -11.6</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>18.6</v>
+        <v>11.6</v>
       </c>
       <c r="P9" t="n">
-        <v>14.5</v>
+        <v>7.5</v>
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -1129,59 +1129,59 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ACC Network</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>34.9</v>
+        <v>26.2</v>
       </c>
       <c r="H10" t="n">
-        <v>23.3</v>
+        <v>27.8</v>
       </c>
       <c r="I10" t="n">
-        <v>74.62</v>
+        <v>40.84</v>
       </c>
       <c r="J10" t="n">
-        <v>3.8</v>
+        <v>9.1</v>
       </c>
       <c r="K10" t="n">
         <v>4.1</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Coastal Carolina -7.5</t>
+          <t>Clemson -2.5</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Coastal Carolina -7.5</t>
+          <t>Clemson -2.5</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Coastal Carolina -11.6</t>
+          <t>Florida State -1.6</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>11.6</v>
+        <v>-1.6</v>
       </c>
       <c r="P10" t="n">
-        <v>7.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
@@ -1269,63 +1269,63 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>8:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>35.4</v>
+        <v>34</v>
       </c>
       <c r="H12" t="n">
-        <v>25.6</v>
+        <v>20.6</v>
       </c>
       <c r="I12" t="n">
-        <v>70.83</v>
+        <v>78.44</v>
       </c>
       <c r="J12" t="n">
-        <v>8.1</v>
+        <v>4.2</v>
       </c>
       <c r="K12" t="n">
-        <v>3.800000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Memphis -6.5</t>
+          <t>Utah State -11.0</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Memphis -6.0</t>
+          <t>Utah State -9.5</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Memphis -9.8</t>
+          <t>Utah State -13.4</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>9.800000000000001</v>
+        <v>13.4</v>
       </c>
       <c r="P12" t="n">
-        <v>6</v>
+        <v>9.5</v>
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
@@ -1341,63 +1341,63 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45966</v>
+        <v>45968</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Kent State</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>28.2</v>
+        <v>35.4</v>
       </c>
       <c r="H13" t="n">
-        <v>23</v>
+        <v>25.6</v>
       </c>
       <c r="I13" t="n">
-        <v>59.7</v>
+        <v>70.83</v>
       </c>
       <c r="J13" t="n">
-        <v>4</v>
+        <v>8.1</v>
       </c>
       <c r="K13" t="n">
-        <v>3.8</v>
+        <v>3.800000000000001</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Ball State -2.5</t>
+          <t>Memphis -6.5</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Ball State -1.5</t>
+          <t>Memphis -6.0</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Ball State -5.3</t>
+          <t>Memphis -9.8</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>5.3</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="P13" t="n">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1427,49 +1427,49 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>34</v>
+        <v>28.1</v>
       </c>
       <c r="H14" t="n">
-        <v>20.6</v>
+        <v>33.7</v>
       </c>
       <c r="I14" t="n">
-        <v>78.44</v>
+        <v>31.54</v>
       </c>
       <c r="J14" t="n">
-        <v>4.2</v>
+        <v>7.6</v>
       </c>
       <c r="K14" t="n">
         <v>3.4</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Utah State -11.0</t>
+          <t>Duke -8.5</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Utah State -10.0</t>
+          <t>Duke -9.0</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Utah State -13.4</t>
+          <t>Duke -5.6</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>13.4</v>
+        <v>-5.6</v>
       </c>
       <c r="P14" t="n">
-        <v>10</v>
+        <v>-9</v>
       </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1485,63 +1485,63 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45969</v>
+        <v>45966</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>Kent State</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>24</v>
+        <v>28.2</v>
       </c>
       <c r="H15" t="n">
-        <v>26.2</v>
+        <v>23</v>
       </c>
       <c r="I15" t="n">
-        <v>41.38</v>
+        <v>59.7</v>
       </c>
       <c r="J15" t="n">
-        <v>5.2</v>
+        <v>4</v>
       </c>
       <c r="K15" t="n">
         <v>3.3</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Jacksonville State -1.5</t>
+          <t>Ball State -2.5</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>UTEP -1.0</t>
+          <t>Ball State -2.0</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Jacksonville State -2.3</t>
+          <t>Ball State -5.3</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>-2.3</v>
+        <v>5.3</v>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
@@ -1557,63 +1557,63 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45969</v>
+        <v>45968</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>21.9</v>
+        <v>25</v>
       </c>
       <c r="H16" t="n">
-        <v>30.3</v>
+        <v>22.8</v>
       </c>
       <c r="I16" t="n">
-        <v>25.17</v>
+        <v>51.12</v>
       </c>
       <c r="J16" t="n">
-        <v>4.6</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="K16" t="n">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Louisiana Tech -4.5</t>
+          <t>UCF --0.0</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Louisiana Tech -5.5</t>
+          <t>Houston -1.0</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Louisiana Tech -8.4</t>
+          <t>UCF -2.1</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>-8.4</v>
+        <v>2.1</v>
       </c>
       <c r="P16" t="n">
-        <v>-5.5</v>
+        <v>-1</v>
       </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
@@ -1629,63 +1629,63 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45965</v>
+        <v>45969</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>30.4</v>
+        <v>21.9</v>
       </c>
       <c r="H17" t="n">
-        <v>17.4</v>
+        <v>30.3</v>
       </c>
       <c r="I17" t="n">
-        <v>77.67</v>
+        <v>25.17</v>
       </c>
       <c r="J17" t="n">
-        <v>2.4</v>
+        <v>4.6</v>
       </c>
       <c r="K17" t="n">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Akron -10.0</t>
+          <t>Louisiana Tech -4.5</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Akron -10.5</t>
+          <t>Louisiana Tech -5.5</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Akron -13.0</t>
+          <t>Louisiana Tech -8.4</t>
         </is>
       </c>
       <c r="O17" t="n">
-        <v>13</v>
+        <v>-8.4</v>
       </c>
       <c r="P17" t="n">
-        <v>10.5</v>
+        <v>-5.5</v>
       </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -1705,59 +1705,59 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1:30 PM</t>
+          <t>3:30 PM</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>27.5</v>
+        <v>18</v>
       </c>
       <c r="H18" t="n">
-        <v>27.1</v>
+        <v>31.4</v>
       </c>
       <c r="I18" t="n">
-        <v>47.47</v>
+        <v>16.87</v>
       </c>
       <c r="J18" t="n">
-        <v>8.300000000000001</v>
+        <v>6.8</v>
       </c>
       <c r="K18" t="n">
-        <v>2.4</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Rutgers -1.0</t>
+          <t>Washington -11.0</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Maryland -2.0</t>
+          <t>Washington -11.0</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Rutgers -0.4</t>
+          <t>Washington -13.3</t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>0.4</v>
+        <v>-13.3</v>
       </c>
       <c r="P18" t="n">
-        <v>-2</v>
+        <v>-11</v>
       </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
@@ -1773,63 +1773,63 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45969</v>
+        <v>45967</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3:30 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H19" t="n">
-        <v>31.4</v>
+        <v>28.8</v>
       </c>
       <c r="I19" t="n">
-        <v>16.87</v>
+        <v>57.52</v>
       </c>
       <c r="J19" t="n">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="K19" t="n">
-        <v>2.300000000000001</v>
+        <v>2.2</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Washington -11.0</t>
+          <t>App State -6.0</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Washington -11.0</t>
+          <t>App State -6.5</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Washington -13.3</t>
+          <t>App State -4.3</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>-13.3</v>
+        <v>4.3</v>
       </c>
       <c r="P19" t="n">
-        <v>-11</v>
+        <v>6.5</v>
       </c>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
@@ -1845,63 +1845,63 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45969</v>
+        <v>45965</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3:30 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>26.2</v>
+        <v>27</v>
       </c>
       <c r="H20" t="n">
-        <v>19.8</v>
+        <v>21.8</v>
       </c>
       <c r="I20" t="n">
-        <v>62.11</v>
+        <v>58.89</v>
       </c>
       <c r="J20" t="n">
-        <v>6.8</v>
+        <v>7.3</v>
       </c>
       <c r="K20" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>North Carolina -9.0</t>
+          <t>Ohio -3.5</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>North Carolina -8.5</t>
+          <t>Ohio -3.0</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>North Carolina -6.3</t>
+          <t>Ohio -5.1</t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>6.3</v>
+        <v>5.1</v>
       </c>
       <c r="P20" t="n">
-        <v>8.5</v>
+        <v>3</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
@@ -1917,7 +1917,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45967</v>
+        <v>45969</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1926,54 +1926,54 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>33</v>
+        <v>30.9</v>
       </c>
       <c r="H21" t="n">
-        <v>28.8</v>
+        <v>18.9</v>
       </c>
       <c r="I21" t="n">
-        <v>57.52</v>
+        <v>75.04000000000001</v>
       </c>
       <c r="J21" t="n">
-        <v>6.3</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K21" t="n">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>App State -6.0</t>
+          <t>Alabama -11.0</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>App State -6.5</t>
+          <t>Alabama -10.0</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>App State -4.3</t>
+          <t>Alabama -12.0</t>
         </is>
       </c>
       <c r="O21" t="n">
-        <v>4.3</v>
+        <v>12</v>
       </c>
       <c r="P21" t="n">
-        <v>6.5</v>
+        <v>10</v>
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
@@ -1993,59 +1993,59 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Air Force</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>25.4</v>
+        <v>34.3</v>
       </c>
       <c r="H22" t="n">
-        <v>29.2</v>
+        <v>31.2</v>
       </c>
       <c r="I22" t="n">
-        <v>35.54</v>
+        <v>53.92</v>
       </c>
       <c r="J22" t="n">
-        <v>5.8</v>
+        <v>7.1</v>
       </c>
       <c r="K22" t="n">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Southern Miss -6.0</t>
+          <t>San José State -3.5</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Southern Miss -6.0</t>
+          <t>San José State -5.0</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Southern Miss -3.9</t>
+          <t>San José State -3.1</t>
         </is>
       </c>
       <c r="O22" t="n">
-        <v>-3.9</v>
+        <v>3.1</v>
       </c>
       <c r="P22" t="n">
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
@@ -2061,63 +2061,63 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45965</v>
+        <v>45969</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>27</v>
+        <v>31.4</v>
       </c>
       <c r="H23" t="n">
-        <v>21.8</v>
+        <v>26</v>
       </c>
       <c r="I23" t="n">
-        <v>58.89</v>
+        <v>59.43</v>
       </c>
       <c r="J23" t="n">
-        <v>7.3</v>
+        <v>5.6</v>
       </c>
       <c r="K23" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Ohio -3.5</t>
+          <t>Florida Atlantic -4.5</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Ohio -3.0</t>
+          <t>Florida Atlantic -3.5</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Ohio -5.1</t>
+          <t>Florida Atlantic -5.3</t>
         </is>
       </c>
       <c r="O23" t="n">
-        <v>5.1</v>
+        <v>5.3</v>
       </c>
       <c r="P23" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
@@ -2137,59 +2137,59 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>30.9</v>
+        <v>29.6</v>
       </c>
       <c r="H24" t="n">
-        <v>18.9</v>
+        <v>24.8</v>
       </c>
       <c r="I24" t="n">
-        <v>75.04000000000001</v>
+        <v>58.35</v>
       </c>
       <c r="J24" t="n">
-        <v>9.300000000000001</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K24" t="n">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Alabama -11.0</t>
+          <t>TCU -6.5</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Alabama -10.0</t>
+          <t>TCU -6.5</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Alabama -12.0</t>
+          <t>TCU -4.8</t>
         </is>
       </c>
       <c r="O24" t="n">
-        <v>12</v>
+        <v>4.8</v>
       </c>
       <c r="P24" t="n">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
@@ -2209,59 +2209,59 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Duke</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>28.1</v>
+        <v>20</v>
       </c>
       <c r="H25" t="n">
-        <v>33.7</v>
+        <v>32.8</v>
       </c>
       <c r="I25" t="n">
-        <v>31.54</v>
+        <v>17.67</v>
       </c>
       <c r="J25" t="n">
-        <v>7.6</v>
+        <v>9</v>
       </c>
       <c r="K25" t="n">
-        <v>1.9</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Duke -8.5</t>
+          <t>Indiana -13.5</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Duke -7.5</t>
+          <t>Indiana -14.5</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Duke -5.6</t>
+          <t>Indiana -12.8</t>
         </is>
       </c>
       <c r="O25" t="n">
-        <v>-5.6</v>
+        <v>-12.8</v>
       </c>
       <c r="P25" t="n">
-        <v>-7.5</v>
+        <v>-14.5</v>
       </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -2281,59 +2281,59 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>31.4</v>
+        <v>32.5</v>
       </c>
       <c r="H26" t="n">
-        <v>26</v>
+        <v>25.9</v>
       </c>
       <c r="I26" t="n">
-        <v>59.43</v>
+        <v>63.68</v>
       </c>
       <c r="J26" t="n">
-        <v>5.6</v>
+        <v>8.9</v>
       </c>
       <c r="K26" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Florida Atlantic -4.5</t>
+          <t>Arizona -6.0</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Florida Atlantic -3.5</t>
+          <t>Arizona -5.0</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Florida Atlantic -5.3</t>
+          <t>Arizona -6.6</t>
         </is>
       </c>
       <c r="O26" t="n">
-        <v>5.3</v>
+        <v>6.6</v>
       </c>
       <c r="P26" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
@@ -2353,59 +2353,59 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>29.6</v>
+        <v>26.2</v>
       </c>
       <c r="H27" t="n">
-        <v>24.8</v>
+        <v>25.6</v>
       </c>
       <c r="I27" t="n">
-        <v>58.35</v>
+        <v>47.47</v>
       </c>
       <c r="J27" t="n">
-        <v>9.199999999999999</v>
+        <v>5</v>
       </c>
       <c r="K27" t="n">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>TCU -6.5</t>
+          <t>Eastern Michigan -1.5</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>TCU -6.5</t>
+          <t>Eastern Michigan -2.0</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>TCU -4.8</t>
+          <t>Eastern Michigan -0.5</t>
         </is>
       </c>
       <c r="O27" t="n">
-        <v>4.8</v>
+        <v>0.5</v>
       </c>
       <c r="P27" t="n">
-        <v>6.5</v>
+        <v>2</v>
       </c>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
@@ -2425,59 +2425,59 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>20</v>
+        <v>20.9</v>
       </c>
       <c r="H28" t="n">
-        <v>32.8</v>
+        <v>25.4</v>
       </c>
       <c r="I28" t="n">
-        <v>17.67</v>
+        <v>34.52</v>
       </c>
       <c r="J28" t="n">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="K28" t="n">
-        <v>1.699999999999999</v>
+        <v>1.5</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Indiana -13.5</t>
+          <t>Florida -3.5</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Indiana -14.5</t>
+          <t>Florida -3.0</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Indiana -12.8</t>
+          <t>Florida -4.5</t>
         </is>
       </c>
       <c r="O28" t="n">
-        <v>-12.8</v>
+        <v>-4.5</v>
       </c>
       <c r="P28" t="n">
-        <v>-14.5</v>
+        <v>-3</v>
       </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
@@ -2497,59 +2497,59 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>Hawai'i</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>23.4</v>
+        <v>18.9</v>
       </c>
       <c r="H29" t="n">
-        <v>33</v>
+        <v>27.4</v>
       </c>
       <c r="I29" t="n">
-        <v>23.92</v>
+        <v>25.81</v>
       </c>
       <c r="J29" t="n">
-        <v>8.699999999999999</v>
+        <v>6.1</v>
       </c>
       <c r="K29" t="n">
-        <v>1.699999999999999</v>
+        <v>1.5</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Georgia -7.5</t>
+          <t>San Diego State -4.5</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Georgia -8.0</t>
+          <t>San Diego State -7.0</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Georgia -9.7</t>
+          <t>San Diego State -8.5</t>
         </is>
       </c>
       <c r="O29" t="n">
-        <v>-9.699999999999999</v>
+        <v>-8.5</v>
       </c>
       <c r="P29" t="n">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
@@ -2569,59 +2569,59 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>1:30 PM</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>32.5</v>
+        <v>27.5</v>
       </c>
       <c r="H30" t="n">
-        <v>25.9</v>
+        <v>27.1</v>
       </c>
       <c r="I30" t="n">
-        <v>63.68</v>
+        <v>47.47</v>
       </c>
       <c r="J30" t="n">
-        <v>8.9</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="K30" t="n">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Arizona -6.0</t>
+          <t>Rutgers -1.0</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Arizona -5.0</t>
+          <t>Maryland -1.0</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Arizona -6.6</t>
+          <t>Rutgers -0.4</t>
         </is>
       </c>
       <c r="O30" t="n">
-        <v>6.6</v>
+        <v>0.4</v>
       </c>
       <c r="P30" t="n">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
@@ -2641,59 +2641,59 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="H31" t="n">
-        <v>17.4</v>
+        <v>26.2</v>
       </c>
       <c r="I31" t="n">
-        <v>93.68000000000001</v>
+        <v>41.38</v>
       </c>
       <c r="J31" t="n">
-        <v>6.3</v>
+        <v>5.2</v>
       </c>
       <c r="K31" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Notre Dame -24.5</t>
+          <t>Jacksonville State -1.5</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Notre Dame -25.0</t>
+          <t>Jacksonville State -1.0</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Notre Dame -26.5</t>
+          <t>Jacksonville State -2.3</t>
         </is>
       </c>
       <c r="O31" t="n">
-        <v>26.5</v>
+        <v>-2.3</v>
       </c>
       <c r="P31" t="n">
-        <v>25</v>
+        <v>-1</v>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
@@ -2713,59 +2713,59 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>3:30 PM</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="G32" t="n">
         <v>26.2</v>
       </c>
       <c r="H32" t="n">
-        <v>25.6</v>
+        <v>19.8</v>
       </c>
       <c r="I32" t="n">
-        <v>47.47</v>
+        <v>62.11</v>
       </c>
       <c r="J32" t="n">
-        <v>5</v>
+        <v>6.8</v>
       </c>
       <c r="K32" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Eastern Michigan -1.5</t>
+          <t>North Carolina -9.0</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Eastern Michigan -2.0</t>
+          <t>North Carolina -7.5</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Eastern Michigan -0.5</t>
+          <t>North Carolina -6.3</t>
         </is>
       </c>
       <c r="O32" t="n">
-        <v>0.5</v>
+        <v>6.3</v>
       </c>
       <c r="P32" t="n">
-        <v>2</v>
+        <v>7.5</v>
       </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
@@ -2785,59 +2785,59 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>20.9</v>
+        <v>25.9</v>
       </c>
       <c r="H33" t="n">
-        <v>25.4</v>
+        <v>25.7</v>
       </c>
       <c r="I33" t="n">
-        <v>34.52</v>
+        <v>46.64</v>
       </c>
       <c r="J33" t="n">
-        <v>8.4</v>
+        <v>4.5</v>
       </c>
       <c r="K33" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Florida -3.5</t>
+          <t>Florida International -1.0</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Florida -3.0</t>
+          <t>Florida International -1.0</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Florida -4.5</t>
+          <t>Middle Tennessee -0.2</t>
         </is>
       </c>
       <c r="O33" t="n">
-        <v>-4.5</v>
+        <v>0.2</v>
       </c>
       <c r="P33" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
@@ -2853,63 +2853,63 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45969</v>
+        <v>45967</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>19.8</v>
+        <v>37.8</v>
       </c>
       <c r="H34" t="n">
-        <v>27.2</v>
+        <v>25</v>
       </c>
       <c r="I34" t="n">
-        <v>27.57</v>
+        <v>77.48</v>
       </c>
       <c r="J34" t="n">
-        <v>9.4</v>
+        <v>7.6</v>
       </c>
       <c r="K34" t="n">
-        <v>1.5</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Oregon -6.0</t>
+          <t>South Florida -13.0</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Oregon -6.0</t>
+          <t>South Florida -14.0</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Oregon -7.5</t>
+          <t>South Florida -12.8</t>
         </is>
       </c>
       <c r="O34" t="n">
-        <v>-7.5</v>
+        <v>12.8</v>
       </c>
       <c r="P34" t="n">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
@@ -2929,59 +2929,59 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Hawai'i</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>San Diego State</t>
+          <t>James Madison</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>18.9</v>
+        <v>22.4</v>
       </c>
       <c r="H35" t="n">
-        <v>27.4</v>
+        <v>35.2</v>
       </c>
       <c r="I35" t="n">
-        <v>25.81</v>
+        <v>17.83</v>
       </c>
       <c r="J35" t="n">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="K35" t="n">
-        <v>1.5</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>San Diego State -4.5</t>
+          <t>James Madison -12.5</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>San Diego State -7.0</t>
+          <t>James Madison -14.0</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>San Diego State -8.5</t>
+          <t>James Madison -12.8</t>
         </is>
       </c>
       <c r="O35" t="n">
-        <v>-8.5</v>
+        <v>-12.8</v>
       </c>
       <c r="P35" t="n">
-        <v>-7</v>
+        <v>-14</v>
       </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
@@ -3001,59 +3001,59 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>BTN</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>10.5</v>
+        <v>23.4</v>
       </c>
       <c r="H36" t="n">
-        <v>40.3</v>
+        <v>33</v>
       </c>
       <c r="I36" t="n">
-        <v>3.22</v>
+        <v>23.92</v>
       </c>
       <c r="J36" t="n">
-        <v>5.1</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="K36" t="n">
-        <v>1.300000000000001</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Ohio State -28.5</t>
+          <t>Georgia -7.5</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Ohio State -28.5</t>
+          <t>Georgia -8.5</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Ohio State -29.8</t>
+          <t>Georgia -9.7</t>
         </is>
       </c>
       <c r="O36" t="n">
-        <v>-29.8</v>
+        <v>-9.699999999999999</v>
       </c>
       <c r="P36" t="n">
-        <v>-28.5</v>
+        <v>-8.5</v>
       </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
@@ -3069,63 +3069,63 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45967</v>
+        <v>45969</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>37.8</v>
+        <v>30.8</v>
       </c>
       <c r="H37" t="n">
-        <v>25</v>
+        <v>32.8</v>
       </c>
       <c r="I37" t="n">
-        <v>77.48</v>
+        <v>41.65</v>
       </c>
       <c r="J37" t="n">
-        <v>7.6</v>
+        <v>6.1</v>
       </c>
       <c r="K37" t="n">
-        <v>1.199999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>South Florida -13.0</t>
+          <t>Texas State -2.5</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>South Florida -14.0</t>
+          <t>Texas State -3.0</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>South Florida -12.8</t>
+          <t>Texas State -1.9</t>
         </is>
       </c>
       <c r="O37" t="n">
-        <v>12.8</v>
+        <v>-1.9</v>
       </c>
       <c r="P37" t="n">
-        <v>14</v>
+        <v>-3</v>
       </c>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
@@ -3141,63 +3141,63 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>25</v>
+        <v>30.2</v>
       </c>
       <c r="H38" t="n">
-        <v>22.8</v>
+        <v>21.6</v>
       </c>
       <c r="I38" t="n">
-        <v>51.12</v>
+        <v>67.73</v>
       </c>
       <c r="J38" t="n">
-        <v>8.800000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="K38" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>UCF --0.0</t>
+          <t>Liberty -8.0</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>UCF -1.0</t>
+          <t>Liberty -7.5</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>UCF -2.1</t>
+          <t>Liberty -8.5</t>
         </is>
       </c>
       <c r="O38" t="n">
-        <v>2.1</v>
+        <v>8.5</v>
       </c>
       <c r="P38" t="n">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
@@ -3217,59 +3217,59 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>8:30 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>28.5</v>
+        <v>29.3</v>
       </c>
       <c r="H39" t="n">
-        <v>33.4</v>
+        <v>21.3</v>
       </c>
       <c r="I39" t="n">
-        <v>34.52</v>
+        <v>66.73999999999999</v>
       </c>
       <c r="J39" t="n">
-        <v>5.8</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K39" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>UNLV -6.0</t>
+          <t>Vanderbilt -7.5</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>UNLV -6.0</t>
+          <t>Vanderbilt -7.0</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>UNLV -4.9</t>
+          <t>Vanderbilt -8.0</t>
         </is>
       </c>
       <c r="O39" t="n">
-        <v>-4.9</v>
+        <v>8</v>
       </c>
       <c r="P39" t="n">
-        <v>-6</v>
+        <v>7</v>
       </c>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
@@ -3289,59 +3289,59 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>30.2</v>
+        <v>19.8</v>
       </c>
       <c r="H40" t="n">
-        <v>21.6</v>
+        <v>27.2</v>
       </c>
       <c r="I40" t="n">
-        <v>67.73</v>
+        <v>27.57</v>
       </c>
       <c r="J40" t="n">
-        <v>5.4</v>
+        <v>9.4</v>
       </c>
       <c r="K40" t="n">
         <v>1</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Liberty -8.0</t>
+          <t>Oregon -6.0</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Liberty -7.5</t>
+          <t>Oregon -6.5</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Liberty -8.5</t>
+          <t>Oregon -7.5</t>
         </is>
       </c>
       <c r="O40" t="n">
-        <v>8.5</v>
+        <v>-7.5</v>
       </c>
       <c r="P40" t="n">
-        <v>7.5</v>
+        <v>-6.5</v>
       </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
@@ -3361,59 +3361,59 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Army</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>29.3</v>
+        <v>31</v>
       </c>
       <c r="H41" t="n">
-        <v>21.3</v>
+        <v>23.8</v>
       </c>
       <c r="I41" t="n">
-        <v>66.73999999999999</v>
+        <v>63.68</v>
       </c>
       <c r="J41" t="n">
-        <v>9.300000000000001</v>
+        <v>7</v>
       </c>
       <c r="K41" t="n">
-        <v>1</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Vanderbilt -7.5</t>
+          <t>Army -6.5</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Vanderbilt -7.0</t>
+          <t>Army -6.5</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Vanderbilt -8.0</t>
+          <t>Army -7.2</t>
         </is>
       </c>
       <c r="O41" t="n">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="P41" t="n">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
@@ -3433,59 +3433,59 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>25.9</v>
+        <v>25.4</v>
       </c>
       <c r="H42" t="n">
-        <v>25.7</v>
+        <v>29.2</v>
       </c>
       <c r="I42" t="n">
-        <v>46.64</v>
+        <v>35.54</v>
       </c>
       <c r="J42" t="n">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="K42" t="n">
-        <v>0.8</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Florida International -1.0</t>
+          <t>Southern Miss -6.0</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Middle Tennessee -1.0</t>
+          <t>Southern Miss -4.5</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Middle Tennessee -0.2</t>
+          <t>Southern Miss -3.9</t>
         </is>
       </c>
       <c r="O42" t="n">
-        <v>0.2</v>
+        <v>-3.9</v>
       </c>
       <c r="P42" t="n">
-        <v>1</v>
+        <v>-4.5</v>
       </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
@@ -3501,11 +3501,11 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45969</v>
+        <v>45965</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3515,49 +3515,49 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>31</v>
+        <v>30.4</v>
       </c>
       <c r="H43" t="n">
-        <v>23.8</v>
+        <v>17.4</v>
       </c>
       <c r="I43" t="n">
-        <v>63.68</v>
+        <v>77.67</v>
       </c>
       <c r="J43" t="n">
-        <v>7</v>
+        <v>2.4</v>
       </c>
       <c r="K43" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Army -6.5</t>
+          <t>Akron -10.0</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Army -6.5</t>
+          <t>Akron -12.5</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Army -7.2</t>
+          <t>Akron -13.0</t>
         </is>
       </c>
       <c r="O43" t="n">
-        <v>7.2</v>
+        <v>13</v>
       </c>
       <c r="P43" t="n">
-        <v>6.5</v>
+        <v>12.5</v>
       </c>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
@@ -3577,59 +3577,59 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>1:00 PM</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>UAB</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>22.4</v>
+        <v>30.4</v>
       </c>
       <c r="H44" t="n">
-        <v>35.2</v>
+        <v>27.4</v>
       </c>
       <c r="I44" t="n">
-        <v>17.83</v>
+        <v>54.48</v>
       </c>
       <c r="J44" t="n">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
       <c r="K44" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>James Madison -12.5</t>
+          <t>Rice -3.0</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>James Madison -13.5</t>
+          <t>Rice -2.5</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>James Madison -12.8</t>
+          <t>Rice -2.9</t>
         </is>
       </c>
       <c r="O44" t="n">
-        <v>-12.8</v>
+        <v>2.9</v>
       </c>
       <c r="P44" t="n">
-        <v>-13.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
@@ -3649,59 +3649,59 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>California</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>18.5</v>
+        <v>35.8</v>
       </c>
       <c r="H45" t="n">
-        <v>28</v>
+        <v>15.4</v>
       </c>
       <c r="I45" t="n">
-        <v>23.52</v>
+        <v>88.42</v>
       </c>
       <c r="J45" t="n">
-        <v>3.9</v>
+        <v>6.1</v>
       </c>
       <c r="K45" t="n">
-        <v>0.5</v>
+        <v>0.3999999999999986</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Kennesaw State -7.0</t>
+          <t>Louisville -18.5</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Kennesaw State -10.0</t>
+          <t>Louisville -20.0</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Kennesaw State -9.5</t>
+          <t>Louisville -20.4</t>
         </is>
       </c>
       <c r="O45" t="n">
-        <v>-9.5</v>
+        <v>20.4</v>
       </c>
       <c r="P45" t="n">
-        <v>-10</v>
+        <v>20</v>
       </c>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
@@ -3721,59 +3721,59 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>34.3</v>
+        <v>31.2</v>
       </c>
       <c r="H46" t="n">
-        <v>31.2</v>
+        <v>21.5</v>
       </c>
       <c r="I46" t="n">
-        <v>53.92</v>
+        <v>70.37</v>
       </c>
       <c r="J46" t="n">
-        <v>7.1</v>
+        <v>9.5</v>
       </c>
       <c r="K46" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>San José State -3.5</t>
+          <t>Texas Tech -10.5</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>San José State -3.5</t>
+          <t>Texas Tech -10.0</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>San José State -3.1</t>
+          <t>Texas Tech -9.7</t>
         </is>
       </c>
       <c r="O46" t="n">
-        <v>3.1</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="P46" t="n">
-        <v>3.5</v>
+        <v>10</v>
       </c>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
@@ -3793,59 +3793,59 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>BTN</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>30.4</v>
+        <v>10.5</v>
       </c>
       <c r="H47" t="n">
-        <v>27.4</v>
+        <v>40.3</v>
       </c>
       <c r="I47" t="n">
-        <v>54.48</v>
+        <v>3.22</v>
       </c>
       <c r="J47" t="n">
-        <v>5.7</v>
+        <v>5.1</v>
       </c>
       <c r="K47" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Rice -3.0</t>
+          <t>Ohio State -28.5</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Rice -2.5</t>
+          <t>Ohio State -30.0</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Rice -2.9</t>
+          <t>Ohio State -29.8</t>
         </is>
       </c>
       <c r="O47" t="n">
-        <v>2.9</v>
+        <v>-29.8</v>
       </c>
       <c r="P47" t="n">
-        <v>2.5</v>
+        <v>-30</v>
       </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
@@ -3865,59 +3865,59 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>35.8</v>
+        <v>41</v>
       </c>
       <c r="H48" t="n">
-        <v>15.4</v>
+        <v>12.4</v>
       </c>
       <c r="I48" t="n">
-        <v>88.42</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="J48" t="n">
-        <v>6.1</v>
+        <v>4.8</v>
       </c>
       <c r="K48" t="n">
-        <v>0.3999999999999986</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Louisville -18.5</t>
+          <t>Miami -28.0</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Louisville -20.0</t>
+          <t>Miami -28.5</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Louisville -20.4</t>
+          <t>Miami -28.6</t>
         </is>
       </c>
       <c r="O48" t="n">
-        <v>20.4</v>
+        <v>28.6</v>
       </c>
       <c r="P48" t="n">
-        <v>20</v>
+        <v>28.5</v>
       </c>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
@@ -3937,59 +3937,59 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>31.2</v>
+        <v>36.6</v>
       </c>
       <c r="H49" t="n">
-        <v>21.5</v>
+        <v>16.7</v>
       </c>
       <c r="I49" t="n">
-        <v>70.37</v>
+        <v>88.19</v>
       </c>
       <c r="J49" t="n">
-        <v>9.5</v>
+        <v>2.4</v>
       </c>
       <c r="K49" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Texas Tech -10.5</t>
+          <t>Oregon State -18.5</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Texas Tech -10.0</t>
+          <t>Oregon State -20.0</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Texas Tech -9.7</t>
+          <t>Oregon State -19.9</t>
         </is>
       </c>
       <c r="O49" t="n">
-        <v>9.699999999999999</v>
+        <v>19.9</v>
       </c>
       <c r="P49" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
@@ -4009,59 +4009,59 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>8:30 PM</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>41</v>
+        <v>28.5</v>
       </c>
       <c r="H50" t="n">
-        <v>12.4</v>
+        <v>33.4</v>
       </c>
       <c r="I50" t="n">
-        <v>94.98999999999999</v>
+        <v>34.52</v>
       </c>
       <c r="J50" t="n">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="K50" t="n">
-        <v>0.1000000000000014</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Miami -28.0</t>
+          <t>UNLV -6.0</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Miami -28.5</t>
+          <t>UNLV -5.0</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Miami -28.6</t>
+          <t>UNLV -4.9</t>
         </is>
       </c>
       <c r="O50" t="n">
-        <v>28.6</v>
+        <v>-4.9</v>
       </c>
       <c r="P50" t="n">
-        <v>28.5</v>
+        <v>-5</v>
       </c>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr"/>
@@ -4081,59 +4081,59 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>9:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>36.6</v>
+        <v>44</v>
       </c>
       <c r="H51" t="n">
-        <v>16.7</v>
+        <v>17.4</v>
       </c>
       <c r="I51" t="n">
-        <v>88.19</v>
+        <v>93.68000000000001</v>
       </c>
       <c r="J51" t="n">
-        <v>2.4</v>
+        <v>6.3</v>
       </c>
       <c r="K51" t="n">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Oregon State -18.5</t>
+          <t>Notre Dame -24.5</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Oregon State -20.0</t>
+          <t>Notre Dame -26.5</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Oregon State -19.9</t>
+          <t>Notre Dame -26.5</t>
         </is>
       </c>
       <c r="O51" t="n">
-        <v>19.9</v>
+        <v>26.5</v>
       </c>
       <c r="P51" t="n">
-        <v>20</v>
+        <v>26.5</v>
       </c>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
@@ -4153,7 +4153,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>4:00 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4163,49 +4163,49 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>30.8</v>
+        <v>18.5</v>
       </c>
       <c r="H52" t="n">
-        <v>32.8</v>
+        <v>28</v>
       </c>
       <c r="I52" t="n">
-        <v>41.65</v>
+        <v>23.52</v>
       </c>
       <c r="J52" t="n">
-        <v>6.1</v>
+        <v>3.9</v>
       </c>
       <c r="K52" t="n">
-        <v>0.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Texas State -2.5</t>
+          <t>Kennesaw State -7.0</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Texas State -2.0</t>
+          <t>Kennesaw State -9.5</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>Texas State -1.9</t>
+          <t>Kennesaw State -9.5</t>
         </is>
       </c>
       <c r="O52" t="n">
-        <v>-1.9</v>
+        <v>-9.5</v>
       </c>
       <c r="P52" t="n">
-        <v>-2</v>
+        <v>-9.5</v>
       </c>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>

</xml_diff>